<commit_message>
Campos de Zona y sector en terceros
</commit_message>
<xml_diff>
--- a/public/importacion/Plantilla Terceros.xlsx
+++ b/public/importacion/Plantilla Terceros.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
   <si>
     <t>TipoIdentificacion_idTipoIdentificacion</t>
   </si>
@@ -162,6 +162,30 @@
   </si>
   <si>
     <t>Sisoft - Datos Generales de Proveedores</t>
+  </si>
+  <si>
+    <t>PROV</t>
+  </si>
+  <si>
+    <t>CTE</t>
+  </si>
+  <si>
+    <t>tipoCliente</t>
+  </si>
+  <si>
+    <t>tipoProveedor</t>
+  </si>
+  <si>
+    <t>Zona</t>
+  </si>
+  <si>
+    <t>Sector Empresarial</t>
+  </si>
+  <si>
+    <t>Zona_idZona</t>
+  </si>
+  <si>
+    <t>SectorEmpresa_idSectorEmpresa</t>
   </si>
 </sst>
 </file>
@@ -684,7 +708,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -692,11 +716,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -742,7 +767,19 @@
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="26">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -820,31 +857,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A3:V5" totalsRowShown="0">
-  <autoFilter ref="A3:V5"/>
-  <tableColumns count="22">
-    <tableColumn id="2" name="Tipo Identificacion" dataDxfId="21"/>
-    <tableColumn id="3" name="Documento No." dataDxfId="20"/>
-    <tableColumn id="4" name="Primer Nombre" dataDxfId="19"/>
-    <tableColumn id="5" name="Segundo Nombre" dataDxfId="18"/>
-    <tableColumn id="6" name="Primer Apellido" dataDxfId="17"/>
-    <tableColumn id="7" name="Segundo Apellido" dataDxfId="16"/>
-    <tableColumn id="8" name="Nombre Completo " dataDxfId="15"/>
-    <tableColumn id="9" name="Fecha de Creación" dataDxfId="14"/>
-    <tableColumn id="10" name="Estado" dataDxfId="13"/>
-    <tableColumn id="11" name="Foto" dataDxfId="12"/>
-    <tableColumn id="12" name="Tipo" dataDxfId="11"/>
-    <tableColumn id="13" name="Dirección" dataDxfId="10"/>
-    <tableColumn id="14" name="Ciudad" dataDxfId="9"/>
-    <tableColumn id="15" name="Teléfono" dataDxfId="8"/>
-    <tableColumn id="16" name="Fax" dataDxfId="7"/>
-    <tableColumn id="17" name="Móvil 1" dataDxfId="6"/>
-    <tableColumn id="18" name="Móvil 2" dataDxfId="5"/>
-    <tableColumn id="19" name="Sexo" dataDxfId="4"/>
-    <tableColumn id="20" name="Fecha Nacimiento" dataDxfId="3"/>
-    <tableColumn id="21" name="Correo Electrónico" dataDxfId="2"/>
-    <tableColumn id="22" name="Página Web" dataDxfId="1"/>
-    <tableColumn id="23" name="Cargo" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A3:Z5" totalsRowShown="0">
+  <autoFilter ref="A3:Z5"/>
+  <tableColumns count="26">
+    <tableColumn id="2" name="Tipo Identificacion" dataDxfId="25"/>
+    <tableColumn id="3" name="Documento No." dataDxfId="24"/>
+    <tableColumn id="4" name="Primer Nombre" dataDxfId="23"/>
+    <tableColumn id="5" name="Segundo Nombre" dataDxfId="22"/>
+    <tableColumn id="6" name="Primer Apellido" dataDxfId="21"/>
+    <tableColumn id="7" name="Segundo Apellido" dataDxfId="20"/>
+    <tableColumn id="8" name="Nombre Completo " dataDxfId="19"/>
+    <tableColumn id="24" name="CTE" dataDxfId="2"/>
+    <tableColumn id="1" name="PROV" dataDxfId="3"/>
+    <tableColumn id="9" name="Fecha de Creación" dataDxfId="18"/>
+    <tableColumn id="10" name="Estado" dataDxfId="17"/>
+    <tableColumn id="11" name="Foto" dataDxfId="16"/>
+    <tableColumn id="12" name="Tipo" dataDxfId="15"/>
+    <tableColumn id="13" name="Dirección" dataDxfId="14"/>
+    <tableColumn id="14" name="Ciudad" dataDxfId="13"/>
+    <tableColumn id="15" name="Teléfono" dataDxfId="12"/>
+    <tableColumn id="16" name="Fax" dataDxfId="11"/>
+    <tableColumn id="17" name="Móvil 1" dataDxfId="10"/>
+    <tableColumn id="18" name="Móvil 2" dataDxfId="9"/>
+    <tableColumn id="19" name="Sexo" dataDxfId="8"/>
+    <tableColumn id="20" name="Fecha Nacimiento" dataDxfId="7"/>
+    <tableColumn id="21" name="Correo Electrónico" dataDxfId="6"/>
+    <tableColumn id="22" name="Página Web" dataDxfId="5"/>
+    <tableColumn id="23" name="Cargo" dataDxfId="4"/>
+    <tableColumn id="25" name="Zona" dataDxfId="1"/>
+    <tableColumn id="26" name="Sector Empresarial" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1142,65 +1183,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="20.125" style="3" customWidth="1"/>
     <col min="2" max="2" width="18" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="29.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="13.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="29.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.25" customWidth="1"/>
+    <col min="26" max="26" width="16.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:26" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1221,53 +1268,65 @@
       <c r="G3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="O3" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="V3" s="8" t="s">
+      <c r="X3" s="7" t="s">
         <v>42</v>
       </c>
+      <c r="Y3" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z3" s="10" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="4" spans="1:22" ht="44.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1289,61 +1348,75 @@
       <c r="G4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="O4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V4" s="9" t="s">
+      <c r="X4" s="8" t="s">
         <v>21</v>
       </c>
+      <c r="Y4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="M5" s="4"/>
+      <c r="L5" s="2"/>
+      <c r="O5" s="4"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
     </row>
   </sheetData>
   <sheetProtection sort="0" autoFilter="0"/>
   <mergeCells count="1">
-    <mergeCell ref="A1:V1"/>
+    <mergeCell ref="A1:X1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -1357,13 +1430,13 @@
           <x14:formula1>
             <xm:f>listas!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>R5</xm:sqref>
+          <xm:sqref>T5</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>listas!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>I5</xm:sqref>
+          <xm:sqref>K5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1381,8 +1454,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.625" customWidth="1"/>
+    <col min="2" max="2" width="16.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>